<commit_message>
added last login and other updates
</commit_message>
<xml_diff>
--- a/templates/template.xlsx
+++ b/templates/template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="175">
   <si>
     <t>PLEASE READ THESE INSTRUCTIONS FULLY BEFORE FILLING OUT THIS TEMPLATE</t>
   </si>
@@ -366,9 +366,6 @@
   </si>
   <si>
     <t>assignment</t>
-  </si>
-  <si>
-    <t>Username</t>
   </si>
   <si>
     <t>Account Type</t>
@@ -28930,18 +28927,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A27:E27"/>
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="A29:E29"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="A31:E31"/>
     <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B18:E18"/>
     <mergeCell ref="B23:E23"/>
+    <mergeCell ref="A27:E27"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -29475,7 +29472,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>14</v>
@@ -29487,34 +29484,34 @@
         <v>21</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="O1" s="10"/>
       <c r="P1" s="10"/>
@@ -29531,37 +29528,37 @@
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>128</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>129</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="15" t="s">
         <v>135</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>136</v>
       </c>
       <c r="N2" s="16">
         <v>45659.0</v>
@@ -29569,37 +29566,37 @@
     </row>
     <row r="3">
       <c r="A3" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3" s="14" t="s">
+      <c r="H3" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="I3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="M3" s="15" t="s">
         <v>144</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>145</v>
       </c>
       <c r="N3" s="16">
         <v>45659.0</v>
@@ -29607,37 +29604,37 @@
     </row>
     <row r="4">
       <c r="A4" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="G4" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="I4" s="11" t="s">
+      <c r="J4" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="M4" s="15" t="s">
         <v>154</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>155</v>
       </c>
       <c r="N4" s="16">
         <v>45659.0</v>
@@ -29645,56 +29642,56 @@
     </row>
     <row r="5">
       <c r="A5" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="D5" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="G5" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="G5" s="15" t="s">
-        <v>160</v>
-      </c>
       <c r="H5" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M5" s="17"/>
       <c r="N5" s="16"/>
     </row>
     <row r="6">
       <c r="A6" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>164</v>
-      </c>
       <c r="H6" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M6" s="17"/>
       <c r="N6" s="16"/>
@@ -33733,154 +33730,154 @@
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>